<commit_message>
#456 : Keep on maintaining supported LanguageServer Protocol features.
</commit_message>
<xml_diff>
--- a/TypeCobol.LanguageServer/Documentation/LanguageServerSupportedFeatures.xlsx
+++ b/TypeCobol.LanguageServer/Documentation/LanguageServerSupportedFeatures.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
   <si>
     <t>Language Server features</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>DidChangeConfigurationNotification</t>
-  </si>
-  <si>
-    <t>To be Finished</t>
   </si>
   <si>
     <t>DidChangeWatchedFilesNotification</t>
@@ -472,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,15 +556,15 @@
         <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
@@ -578,7 +575,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Update doc excel for LanguageServer
</commit_message>
<xml_diff>
--- a/TypeCobol.LanguageServer/Documentation/LanguageServerSupportedFeatures.xlsx
+++ b/TypeCobol.LanguageServer/Documentation/LanguageServerSupportedFeatures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAYANJE\Source\Repos\TypeCobol9\TypeCobol\TypeCobol.LanguageServer\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COLLARBE\Source\Repos\TypeCobol\TypeCobol.LanguageServer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -470,7 +470,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +570,7 @@
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
#456: Update doc excel for LanguageServer
</commit_message>
<xml_diff>
--- a/TypeCobol.LanguageServer/Documentation/LanguageServerSupportedFeatures.xlsx
+++ b/TypeCobol.LanguageServer/Documentation/LanguageServerSupportedFeatures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COLLARBE\Source\Repos\TypeCobol\TypeCobol.LanguageServer\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAYANJE\Source\Repos\TypeCobol9\TypeCobol\TypeCobol.LanguageServer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +567,7 @@
         <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>

</xml_diff>